<commit_message>
RR - CEB Meeting
</commit_message>
<xml_diff>
--- a/scripts/station_info.xlsx
+++ b/scripts/station_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rebecca Ruiz\Documents\fish_biodiversity\scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbird\Downloads\fish_biodiversity\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E0F5756-229C-4ACF-ACB9-854F5C17C3B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E0623B9-64ED-4E98-B02C-AA113143A623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="15196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3513" yWindow="2567" windowWidth="17134" windowHeight="10033" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="station_info" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Christopher Bird:</t>
         </r>
@@ -55,7 +55,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 this column was made by Rebecca Ruiz, it is a combination of information from the database query (on the left) and the field data records</t>
@@ -94,7 +94,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Christopher Bird:</t>
         </r>
@@ -103,7 +103,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 word for word, the method of capture field from the field data records</t>
@@ -118,7 +118,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Christopher Bird:</t>
         </r>
@@ -127,7 +127,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 made by Rebecca Ruiz, inferredf from method_capture</t>
@@ -142,7 +142,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Christopher Bird:</t>
         </r>
@@ -151,10 +151,34 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 sum of volumes from method_capture column</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AC30" authorId="0" shapeId="0" xr:uid="{F1E68B56-9488-4C53-BF90-1CF582B33A0C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Christopher Bird:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+handwriting hard to interpret </t>
         </r>
       </text>
     </comment>
@@ -2157,7 +2181,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2304,19 +2328,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="35">
@@ -2672,7 +2683,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -2680,6 +2691,18 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3051,119 +3074,117 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="X1" activePane="topRight" state="frozen"/>
-      <selection activeCell="U1" sqref="U1"/>
-      <selection pane="topRight" activeCell="AC43" sqref="AC43"/>
+    <sheetView tabSelected="1" topLeftCell="W16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W42" sqref="A42:XFD42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="21" width="9" style="2"/>
-    <col min="22" max="23" width="9.1328125" style="2" customWidth="1"/>
+    <col min="22" max="23" width="9.1171875" style="2" customWidth="1"/>
     <col min="24" max="24" width="9" style="1"/>
-    <col min="25" max="28" width="9.1328125" customWidth="1"/>
+    <col min="25" max="28" width="9.1171875" customWidth="1"/>
     <col min="29" max="29" width="22" customWidth="1"/>
-    <col min="30" max="30" width="24.1328125" customWidth="1"/>
-    <col min="31" max="31" width="9.1328125" style="4" customWidth="1"/>
+    <col min="30" max="30" width="24.1171875" customWidth="1"/>
+    <col min="31" max="31" width="9.1171875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:37" s="9" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="8" t="s">
         <v>618</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Y1" s="9" t="s">
         <v>454</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="Z1" s="9" t="s">
         <v>455</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AA1" s="9" t="s">
         <v>456</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AB1" s="9" t="s">
         <v>459</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AC1" s="9" t="s">
         <v>457</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AD1" s="9" t="s">
         <v>617</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AE1" s="10" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
         <v>309</v>
       </c>
@@ -3258,7 +3279,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
         <v>314</v>
       </c>
@@ -3353,7 +3374,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="s">
         <v>321</v>
       </c>
@@ -3448,7 +3469,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.5">
       <c r="A5" s="2" t="s">
         <v>328</v>
       </c>
@@ -3543,7 +3564,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.5">
       <c r="A6" s="2" t="s">
         <v>331</v>
       </c>
@@ -3638,7 +3659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.5">
       <c r="A7" s="2" t="s">
         <v>335</v>
       </c>
@@ -3733,7 +3754,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A8" s="2" t="s">
         <v>340</v>
       </c>
@@ -3833,7 +3854,7 @@
       <c r="AJ8"/>
       <c r="AK8"/>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.5">
       <c r="A9" s="2" t="s">
         <v>346</v>
       </c>
@@ -3928,7 +3949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.5">
       <c r="A10" s="2" t="s">
         <v>350</v>
       </c>
@@ -4023,7 +4044,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.5">
       <c r="A11" s="2" t="s">
         <v>358</v>
       </c>
@@ -4118,7 +4139,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.5">
       <c r="A12" s="2" t="s">
         <v>364</v>
       </c>
@@ -4213,7 +4234,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.5">
       <c r="A13" s="2" t="s">
         <v>370</v>
       </c>
@@ -4308,7 +4329,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.5">
       <c r="A14" s="2" t="s">
         <v>449</v>
       </c>
@@ -4403,7 +4424,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.5">
       <c r="A15" s="2" t="s">
         <v>375</v>
       </c>
@@ -4498,7 +4519,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.5">
       <c r="A16" s="2" t="s">
         <v>380</v>
       </c>
@@ -4593,7 +4614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A17" s="2" t="s">
         <v>385</v>
       </c>
@@ -4689,7 +4710,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A18" s="2" t="s">
         <v>390</v>
       </c>
@@ -4784,7 +4805,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A19" s="2" t="s">
         <v>395</v>
       </c>
@@ -4879,7 +4900,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A20" s="2" t="s">
         <v>401</v>
       </c>
@@ -4974,7 +4995,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A21" s="2" t="s">
         <v>406</v>
       </c>
@@ -5069,7 +5090,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A22" s="2" t="s">
         <v>411</v>
       </c>
@@ -5164,7 +5185,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A23" s="2" t="s">
         <v>416</v>
       </c>
@@ -5259,7 +5280,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A24" s="2" t="s">
         <v>421</v>
       </c>
@@ -5354,7 +5375,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A25" s="2" t="s">
         <v>426</v>
       </c>
@@ -5449,7 +5470,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A26" s="2" t="s">
         <v>432</v>
       </c>
@@ -5544,7 +5565,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A27" s="2" t="s">
         <v>439</v>
       </c>
@@ -5639,7 +5660,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A28" s="2" t="s">
         <v>444</v>
       </c>
@@ -5734,7 +5755,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A29" s="2" t="s">
         <v>47</v>
       </c>
@@ -5829,7 +5850,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A30" s="2" t="s">
         <v>54</v>
       </c>
@@ -5924,7 +5945,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A31" s="2" t="s">
         <v>63</v>
       </c>
@@ -6019,7 +6040,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A32" s="2" t="s">
         <v>68</v>
       </c>
@@ -6114,7 +6135,7 @@
         <v>5.25</v>
       </c>
     </row>
-    <row r="33" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A33" s="2" t="s">
         <v>74</v>
       </c>
@@ -6209,7 +6230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A34" s="2" t="s">
         <v>79</v>
       </c>
@@ -6304,7 +6325,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A35" s="2" t="s">
         <v>84</v>
       </c>
@@ -6399,7 +6420,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A36" s="2" t="s">
         <v>89</v>
       </c>
@@ -6494,7 +6515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A37" s="2" t="s">
         <v>93</v>
       </c>
@@ -6589,7 +6610,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A38" s="2" t="s">
         <v>93</v>
       </c>
@@ -6684,7 +6705,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="39" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A39" s="2" t="s">
         <v>104</v>
       </c>
@@ -6779,7 +6800,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A40" s="2" t="s">
         <v>110</v>
       </c>
@@ -6874,7 +6895,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A41" s="2" t="s">
         <v>35</v>
       </c>
@@ -6969,7 +6990,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A42" s="2" t="s">
         <v>35</v>
       </c>
@@ -7064,7 +7085,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A43" s="2" t="s">
         <v>120</v>
       </c>
@@ -7159,7 +7180,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A44" s="2" t="s">
         <v>125</v>
       </c>
@@ -7254,7 +7275,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A45" s="2" t="s">
         <v>129</v>
       </c>
@@ -7349,7 +7370,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A46" s="3">
         <v>28636</v>
       </c>
@@ -7444,7 +7465,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A47" s="2" t="s">
         <v>138</v>
       </c>
@@ -7539,7 +7560,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A48" s="2" t="s">
         <v>142</v>
       </c>
@@ -7634,7 +7655,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="49" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A49" s="2" t="s">
         <v>146</v>
       </c>
@@ -7729,7 +7750,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A50" s="2" t="s">
         <v>153</v>
       </c>
@@ -7824,7 +7845,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A51" s="2" t="s">
         <v>159</v>
       </c>
@@ -7919,7 +7940,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A52" s="2" t="s">
         <v>164</v>
       </c>
@@ -8014,7 +8035,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="53" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A53" s="2" t="s">
         <v>169</v>
       </c>
@@ -8109,7 +8130,7 @@
         <v>2.33</v>
       </c>
     </row>
-    <row r="54" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A54" s="2" t="s">
         <v>174</v>
       </c>
@@ -8204,7 +8225,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="55" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A55" s="2" t="s">
         <v>180</v>
       </c>
@@ -8299,7 +8320,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A56" s="2" t="s">
         <v>186</v>
       </c>
@@ -8394,7 +8415,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A57" s="2" t="s">
         <v>191</v>
       </c>
@@ -8489,7 +8510,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A58" s="2" t="s">
         <v>198</v>
       </c>
@@ -8584,7 +8605,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A59" s="2" t="s">
         <v>23</v>
       </c>
@@ -8680,7 +8701,7 @@
         <v>9.75</v>
       </c>
     </row>
-    <row r="60" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A60" s="2" t="s">
         <v>202</v>
       </c>
@@ -8775,7 +8796,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A61" s="2" t="s">
         <v>207</v>
       </c>
@@ -8870,7 +8891,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="62" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A62" s="2" t="s">
         <v>215</v>
       </c>
@@ -8965,7 +8986,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="63" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A63" s="2" t="s">
         <v>220</v>
       </c>
@@ -9060,7 +9081,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="64" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A64" s="2" t="s">
         <v>225</v>
       </c>
@@ -9155,7 +9176,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A65" s="2" t="s">
         <v>230</v>
       </c>
@@ -9250,7 +9271,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="66" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A66" s="2" t="s">
         <v>238</v>
       </c>
@@ -9345,7 +9366,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="67" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A67" s="2" t="s">
         <v>243</v>
       </c>
@@ -9440,7 +9461,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="68" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A68" s="2" t="s">
         <v>247</v>
       </c>
@@ -9535,7 +9556,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A69" s="2" t="s">
         <v>252</v>
       </c>
@@ -9630,7 +9651,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="70" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A70" s="2" t="s">
         <v>258</v>
       </c>
@@ -9725,7 +9746,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="71" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A71" s="2" t="s">
         <v>263</v>
       </c>
@@ -9820,7 +9841,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="72" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A72" s="2" t="s">
         <v>269</v>
       </c>
@@ -9915,7 +9936,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="73" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A73" s="2" t="s">
         <v>275</v>
       </c>
@@ -10010,7 +10031,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="74" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A74" s="2" t="s">
         <v>280</v>
       </c>
@@ -10105,7 +10126,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="75" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A75" s="2" t="s">
         <v>286</v>
       </c>
@@ -10200,7 +10221,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="76" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A76" s="2" t="s">
         <v>280</v>
       </c>
@@ -10295,7 +10316,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="77" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A77" s="2" t="s">
         <v>280</v>
       </c>
@@ -10390,7 +10411,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="78" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A78" s="2" t="s">
         <v>304</v>
       </c>
@@ -10485,7 +10506,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="79" spans="1:31" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:31" x14ac:dyDescent="0.5">
       <c r="A79" s="2" t="s">
         <v>299</v>
       </c>
@@ -10585,7 +10606,7 @@
     <sortCondition ref="U2:U79"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>